<commit_message>
docs file menu test
</commit_message>
<xml_diff>
--- a/selenium-web-driver/отчет.xlsx
+++ b/selenium-web-driver/отчет.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\project\software-testing\selenium-web-driver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CA718E4-92E0-4B63-9C91-B8C1392D8166}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C8AE04-15E6-4EFF-B693-22226493C26A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{88CBF015-8B08-482D-A2E4-85EF0F3FCC95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{88CBF015-8B08-482D-A2E4-85EF0F3FCC95}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="13">
   <si>
     <t>id</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Figures test</t>
+  </si>
+  <si>
+    <t>Text area test</t>
+  </si>
+  <si>
+    <t>такое себе</t>
   </si>
 </sst>
 </file>
@@ -416,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACA9620C-F64B-481D-A47E-500F6A49A507}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -427,7 +433,7 @@
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -441,7 +447,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -455,7 +461,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -469,7 +475,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -483,7 +489,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -497,7 +503,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -511,7 +517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -521,13 +527,28 @@
       <c r="C7" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>

</xml_diff>